<commit_message>
updated examples with new field
</commit_message>
<xml_diff>
--- a/examples/etl_example.xlsx
+++ b/examples/etl_example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
   <si>
     <t>SOURCE_SERVER</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>D_LION_PropertyValue_ID;[varchar(80)] NOT NULL;S_LION.Get_LionPropertyValue_ID(source.PropertyDefinitionId, source.EntityTypeId, source.NewValue)|D_LION_PropertyValue_ID;[varchar(80)] NOT NULL;S_LION.Get_LionPropertyValue_ID(source.PropertyDefinitionId, source.EntityTypeId, source.NewValue)</t>
+  </si>
+  <si>
+    <t>USER_REFINED_PK</t>
   </si>
 </sst>
 </file>
@@ -536,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -567,9 +570,10 @@
     <col min="22" max="22" width="31.5" customWidth="1"/>
     <col min="23" max="23" width="14.33203125" customWidth="1"/>
     <col min="24" max="24" width="15.83203125" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -642,8 +646,11 @@
       <c r="X1" t="s">
         <v>19</v>
       </c>
+      <c r="Y1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -708,7 +715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -770,7 +777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -832,7 +839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Updated code to handle specifying the source table pk
</commit_message>
<xml_diff>
--- a/examples/etl_example.xlsx
+++ b/examples/etl_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32920" yWindow="-660" windowWidth="28800" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="-33600" yWindow="-3000" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,10 +144,10 @@
     <t>D_LION_PropertyValue_ID;[varchar(80)] NOT NULL;S_LION.Get_LionPropertyValue_ID(source.PropertyDefinitionId, source.EntityTypeId, source.NewValue)|D_LION_PropertyValue_ID;[varchar(80)] NOT NULL;S_LION.Get_LionPropertyValue_ID(source.PropertyDefinitionId, source.EntityTypeId, source.NewValue)</t>
   </si>
   <si>
-    <t>USER_REFINED_PK</t>
-  </si>
-  <si>
     <t>UPDATE_DTTM|INSERT_DTTM</t>
+  </si>
+  <si>
+    <t>SOURCE_TABLE_PRIMARY_KEY</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,24 +553,23 @@
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="38.1640625" customWidth="1"/>
     <col min="7" max="7" width="37.1640625" customWidth="1"/>
-    <col min="8" max="8" width="38.5" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="23.5" customWidth="1"/>
-    <col min="13" max="13" width="35" customWidth="1"/>
-    <col min="14" max="14" width="51" customWidth="1"/>
-    <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="31.1640625" customWidth="1"/>
-    <col min="17" max="17" width="21.6640625" customWidth="1"/>
-    <col min="18" max="18" width="31.1640625" customWidth="1"/>
-    <col min="19" max="19" width="25.5" customWidth="1"/>
-    <col min="20" max="20" width="33.6640625" customWidth="1"/>
-    <col min="21" max="21" width="31.33203125" customWidth="1"/>
-    <col min="22" max="22" width="31.5" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" customWidth="1"/>
-    <col min="24" max="24" width="15.83203125" customWidth="1"/>
-    <col min="25" max="25" width="21.1640625" customWidth="1"/>
+    <col min="8" max="9" width="38.5" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="23.5" customWidth="1"/>
+    <col min="14" max="14" width="35" customWidth="1"/>
+    <col min="15" max="15" width="51" customWidth="1"/>
+    <col min="16" max="16" width="30" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" customWidth="1"/>
+    <col min="19" max="19" width="31.1640625" customWidth="1"/>
+    <col min="20" max="20" width="25.5" customWidth="1"/>
+    <col min="21" max="21" width="33.6640625" customWidth="1"/>
+    <col min="22" max="22" width="31.33203125" customWidth="1"/>
+    <col min="23" max="23" width="31.5" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" customWidth="1"/>
+    <col min="25" max="25" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -599,55 +598,55 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>37</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -675,43 +674,43 @@
       <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>40</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>28</v>
       </c>
-      <c r="T2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2">
+      <c r="U2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2">
         <v>15</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>1440</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>1</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -740,40 +739,40 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>30</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>27</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="T3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3">
+      <c r="U3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3">
         <v>15</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>1440</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>1</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -802,40 +801,40 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>31</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>27</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>34</v>
       </c>
-      <c r="T4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4">
+      <c r="U4" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4">
         <v>15</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>1440</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>1</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -864,40 +863,40 @@
       <c r="H5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>21</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>27</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>35</v>
       </c>
-      <c r="T5" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5">
+      <c r="U5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5">
         <v>15</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>1440</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated examples to include the new key
</commit_message>
<xml_diff>
--- a/examples/etl_example.xlsx
+++ b/examples/etl_example.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincechavez/Work/UMA_DATA/ETL_AUTOMATION/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A1C4B-AB29-8D49-A20E-16E0F0F5671F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="-3000" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>SOURCE_SERVER</t>
   </si>
@@ -148,12 +154,15 @@
   </si>
   <si>
     <t>SOURCE_TABLE_PRIMARY_KEY</t>
+  </si>
+  <si>
+    <t>SOURCE_EXCLUDED_COLUMNS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -214,6 +223,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -538,14 +555,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="3" width="20.5" customWidth="1"/>
@@ -553,26 +570,26 @@
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="38.1640625" customWidth="1"/>
     <col min="7" max="7" width="37.1640625" customWidth="1"/>
-    <col min="8" max="9" width="38.5" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="23.5" customWidth="1"/>
-    <col min="14" max="14" width="35" customWidth="1"/>
-    <col min="15" max="15" width="51" customWidth="1"/>
-    <col min="16" max="16" width="30" customWidth="1"/>
-    <col min="17" max="17" width="31.1640625" customWidth="1"/>
-    <col min="18" max="18" width="21.6640625" customWidth="1"/>
-    <col min="19" max="19" width="31.1640625" customWidth="1"/>
-    <col min="20" max="20" width="25.5" customWidth="1"/>
-    <col min="21" max="21" width="33.6640625" customWidth="1"/>
-    <col min="22" max="22" width="31.33203125" customWidth="1"/>
-    <col min="23" max="23" width="31.5" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" customWidth="1"/>
-    <col min="25" max="25" width="15.83203125" customWidth="1"/>
+    <col min="8" max="10" width="38.5" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="15" width="35" customWidth="1"/>
+    <col min="16" max="16" width="51" customWidth="1"/>
+    <col min="17" max="17" width="30" customWidth="1"/>
+    <col min="18" max="18" width="31.1640625" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" customWidth="1"/>
+    <col min="20" max="20" width="31.1640625" customWidth="1"/>
+    <col min="21" max="21" width="25.5" customWidth="1"/>
+    <col min="22" max="22" width="33.6640625" customWidth="1"/>
+    <col min="23" max="23" width="31.33203125" customWidth="1"/>
+    <col min="24" max="24" width="31.5" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,55 +618,58 @@
         <v>42</v>
       </c>
       <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -674,47 +694,47 @@
       <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>27</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>28</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>41</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>15</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>1440</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>1</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -739,44 +759,44 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>27</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>27</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>33</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>41</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>15</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>1440</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>1</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -801,44 +821,44 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>27</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>27</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>34</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>41</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>15</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>1440</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>1</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -863,40 +883,40 @@
       <c r="H5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>32</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>27</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>27</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>35</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>41</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>15</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1440</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>1</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug handling the sps
</commit_message>
<xml_diff>
--- a/examples/etl_example.xlsx
+++ b/examples/etl_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincechavez/Work/UMA_DATA/ETL_AUTOMATION/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A1C4B-AB29-8D49-A20E-16E0F0F5671F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EFAD5B-996F-E441-8295-6611CF99CFAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>SOURCE_SERVER</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>SOURCE_EXCLUDED_COLUMNS</t>
+  </si>
+  <si>
+    <t>AgentActivityLog</t>
+  </si>
+  <si>
+    <t>I3TimeStampGMT</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,7 +710,7 @@
         <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
@@ -766,7 +775,7 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
         <v>30</v>
@@ -828,7 +837,7 @@
         <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
         <v>31</v>
@@ -890,7 +899,7 @@
         <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="N5" t="s">
         <v>32</v>
@@ -918,6 +927,50 @@
       </c>
       <c r="Z5" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>